<commit_message>
New data file for manipulated fitness experiment pupae emergence.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_pupae.xlsx
+++ b/data/fitness_development/MFE_pupae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F357DD02-9D71-1A44-81D2-4CC95E88A9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABA6EEA5-1D27-724C-90D4-AC1C821C3DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4676CD7-2E49-4B49-A091-3E192C473528}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="6">
   <si>
     <t>vial</t>
   </si>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C1B781-7514-9640-96DE-98CFCBD1D8E4}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1701,6 +1701,840 @@
         <v>0</v>
       </c>
     </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>196</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93">
+        <v>196</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>196</v>
+      </c>
+      <c r="D94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95">
+        <v>196</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96">
+        <v>196</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97">
+        <v>196</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>196</v>
+      </c>
+      <c r="D98">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>4</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>196</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>196</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>196</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>6</v>
+      </c>
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>196</v>
+      </c>
+      <c r="D102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>6</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>196</v>
+      </c>
+      <c r="D103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>7</v>
+      </c>
+      <c r="B104" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>196</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105">
+        <v>196</v>
+      </c>
+      <c r="D105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106">
+        <v>196</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>8</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107">
+        <v>196</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>9</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108">
+        <v>196</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>9</v>
+      </c>
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109">
+        <v>196</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>10</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <v>196</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>10</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111">
+        <v>196</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>11</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112">
+        <v>196</v>
+      </c>
+      <c r="D112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>11</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113">
+        <v>196</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>12</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114">
+        <v>196</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115">
+        <v>196</v>
+      </c>
+      <c r="D115">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>13</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116">
+        <v>196</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>13</v>
+      </c>
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117">
+        <v>196</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>15</v>
+      </c>
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118">
+        <v>196</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>14</v>
+      </c>
+      <c r="B119" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119">
+        <v>196</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>15</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>15</v>
+      </c>
+      <c r="B121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121">
+        <v>196</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122">
+        <v>212</v>
+      </c>
+      <c r="D122">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123">
+        <v>212</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>2</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124">
+        <v>212</v>
+      </c>
+      <c r="D124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>2</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125">
+        <v>212</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <v>212</v>
+      </c>
+      <c r="D126">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>3</v>
+      </c>
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127">
+        <v>212</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>4</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128">
+        <v>212</v>
+      </c>
+      <c r="D128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>4</v>
+      </c>
+      <c r="B129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129">
+        <v>212</v>
+      </c>
+      <c r="D129">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>212</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131">
+        <v>212</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>6</v>
+      </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132">
+        <v>212</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>6</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
+        <v>212</v>
+      </c>
+      <c r="D133">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>7</v>
+      </c>
+      <c r="B134" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134">
+        <v>212</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>7</v>
+      </c>
+      <c r="B135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135">
+        <v>212</v>
+      </c>
+      <c r="D135">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>8</v>
+      </c>
+      <c r="B136" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>212</v>
+      </c>
+      <c r="D136">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>8</v>
+      </c>
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137">
+        <v>212</v>
+      </c>
+      <c r="D137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>9</v>
+      </c>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138">
+        <v>212</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>9</v>
+      </c>
+      <c r="B139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139">
+        <v>212</v>
+      </c>
+      <c r="D139">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>10</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140">
+        <v>212</v>
+      </c>
+      <c r="D140">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>10</v>
+      </c>
+      <c r="B141" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>212</v>
+      </c>
+      <c r="D141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>11</v>
+      </c>
+      <c r="B142" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142">
+        <v>212</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>11</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>212</v>
+      </c>
+      <c r="D143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>12</v>
+      </c>
+      <c r="B144" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144">
+        <v>212</v>
+      </c>
+      <c r="D144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>12</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145">
+        <v>212</v>
+      </c>
+      <c r="D145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>13</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146">
+        <v>212</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>13</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>212</v>
+      </c>
+      <c r="D147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>15</v>
+      </c>
+      <c r="B148" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148">
+        <v>212</v>
+      </c>
+      <c r="D148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>14</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149">
+        <v>212</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>15</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>15</v>
+      </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151">
+        <v>212</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the manipulated fitness experiment with new data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_pupae.xlsx
+++ b/data/fitness_development/MFE_pupae.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_17/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92A639E-90DA-C54E-B64C-E5EC72B69203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB1EA14F-7B5D-AA42-96E1-5692AFD81E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4676CD7-2E49-4B49-A091-3E192C473528}"/>
+    <workbookView xWindow="1200" yWindow="540" windowWidth="28800" windowHeight="16100" xr2:uid="{C4676CD7-2E49-4B49-A091-3E192C473528}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="6">
   <si>
     <t>vial</t>
   </si>
@@ -89,9 +89,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C1B781-7514-9640-96DE-98CFCBD1D8E4}">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D261" sqref="D261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,7 +2033,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="1">
+      <c r="A115">
         <v>14</v>
       </c>
       <c r="B115" t="s">
@@ -3291,6 +3290,812 @@
       </c>
       <c r="D204">
         <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>1</v>
+      </c>
+      <c r="B205" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205">
+        <v>245</v>
+      </c>
+      <c r="D205">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>1</v>
+      </c>
+      <c r="B206" t="s">
+        <v>5</v>
+      </c>
+      <c r="C206">
+        <v>245</v>
+      </c>
+      <c r="D206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>2</v>
+      </c>
+      <c r="B207" t="s">
+        <v>4</v>
+      </c>
+      <c r="C207">
+        <v>245</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>2</v>
+      </c>
+      <c r="B208" t="s">
+        <v>5</v>
+      </c>
+      <c r="C208">
+        <v>245</v>
+      </c>
+      <c r="D208">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>3</v>
+      </c>
+      <c r="B209" t="s">
+        <v>4</v>
+      </c>
+      <c r="C209">
+        <v>245</v>
+      </c>
+      <c r="D209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>5</v>
+      </c>
+      <c r="C210">
+        <v>245</v>
+      </c>
+      <c r="D210">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>4</v>
+      </c>
+      <c r="B211" t="s">
+        <v>4</v>
+      </c>
+      <c r="C211">
+        <v>245</v>
+      </c>
+      <c r="D211">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>4</v>
+      </c>
+      <c r="B212" t="s">
+        <v>5</v>
+      </c>
+      <c r="C212">
+        <v>245</v>
+      </c>
+      <c r="D212">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>5</v>
+      </c>
+      <c r="B213" t="s">
+        <v>4</v>
+      </c>
+      <c r="C213">
+        <v>245</v>
+      </c>
+      <c r="D213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>5</v>
+      </c>
+      <c r="B214" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214">
+        <v>245</v>
+      </c>
+      <c r="D214">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>6</v>
+      </c>
+      <c r="B215" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215">
+        <v>245</v>
+      </c>
+      <c r="D215">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>6</v>
+      </c>
+      <c r="B216" t="s">
+        <v>5</v>
+      </c>
+      <c r="C216">
+        <v>245</v>
+      </c>
+      <c r="D216">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>7</v>
+      </c>
+      <c r="B217" t="s">
+        <v>4</v>
+      </c>
+      <c r="C217">
+        <v>245</v>
+      </c>
+      <c r="D217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>7</v>
+      </c>
+      <c r="B218" t="s">
+        <v>5</v>
+      </c>
+      <c r="C218">
+        <v>245</v>
+      </c>
+      <c r="D218">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>8</v>
+      </c>
+      <c r="B219" t="s">
+        <v>4</v>
+      </c>
+      <c r="C219">
+        <v>245</v>
+      </c>
+      <c r="D219">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>8</v>
+      </c>
+      <c r="B220" t="s">
+        <v>5</v>
+      </c>
+      <c r="C220">
+        <v>245</v>
+      </c>
+      <c r="D220">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>9</v>
+      </c>
+      <c r="B221" t="s">
+        <v>4</v>
+      </c>
+      <c r="C221">
+        <v>245</v>
+      </c>
+      <c r="D221">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>9</v>
+      </c>
+      <c r="B222" t="s">
+        <v>5</v>
+      </c>
+      <c r="C222">
+        <v>245</v>
+      </c>
+      <c r="D222">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>10</v>
+      </c>
+      <c r="B223" t="s">
+        <v>4</v>
+      </c>
+      <c r="C223">
+        <v>245</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>10</v>
+      </c>
+      <c r="B224" t="s">
+        <v>5</v>
+      </c>
+      <c r="C224">
+        <v>245</v>
+      </c>
+      <c r="D224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>11</v>
+      </c>
+      <c r="B225" t="s">
+        <v>4</v>
+      </c>
+      <c r="C225">
+        <v>245</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>11</v>
+      </c>
+      <c r="B226" t="s">
+        <v>5</v>
+      </c>
+      <c r="C226">
+        <v>245</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>12</v>
+      </c>
+      <c r="B227" t="s">
+        <v>4</v>
+      </c>
+      <c r="C227">
+        <v>245</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>12</v>
+      </c>
+      <c r="B228" t="s">
+        <v>5</v>
+      </c>
+      <c r="C228">
+        <v>245</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229" t="s">
+        <v>4</v>
+      </c>
+      <c r="C229">
+        <v>245</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>13</v>
+      </c>
+      <c r="B230" t="s">
+        <v>5</v>
+      </c>
+      <c r="C230">
+        <v>245</v>
+      </c>
+      <c r="D230">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>14</v>
+      </c>
+      <c r="B231" t="s">
+        <v>4</v>
+      </c>
+      <c r="C231">
+        <v>245</v>
+      </c>
+      <c r="D231">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>14</v>
+      </c>
+      <c r="B232" t="s">
+        <v>5</v>
+      </c>
+      <c r="C232">
+        <v>245</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>15</v>
+      </c>
+      <c r="B233" t="s">
+        <v>5</v>
+      </c>
+      <c r="C233">
+        <v>245</v>
+      </c>
+      <c r="D233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>1</v>
+      </c>
+      <c r="B234" t="s">
+        <v>4</v>
+      </c>
+      <c r="C234">
+        <v>260</v>
+      </c>
+      <c r="D234">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>1</v>
+      </c>
+      <c r="B235" t="s">
+        <v>5</v>
+      </c>
+      <c r="C235">
+        <v>260</v>
+      </c>
+      <c r="D235">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>2</v>
+      </c>
+      <c r="B236" t="s">
+        <v>4</v>
+      </c>
+      <c r="C236">
+        <v>260</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>2</v>
+      </c>
+      <c r="B237" t="s">
+        <v>5</v>
+      </c>
+      <c r="C237">
+        <v>260</v>
+      </c>
+      <c r="D237">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238">
+        <v>260</v>
+      </c>
+      <c r="D238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>3</v>
+      </c>
+      <c r="B239" t="s">
+        <v>5</v>
+      </c>
+      <c r="C239">
+        <v>260</v>
+      </c>
+      <c r="D239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>4</v>
+      </c>
+      <c r="B240" t="s">
+        <v>4</v>
+      </c>
+      <c r="C240">
+        <v>260</v>
+      </c>
+      <c r="D240">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>4</v>
+      </c>
+      <c r="B241" t="s">
+        <v>5</v>
+      </c>
+      <c r="C241">
+        <v>260</v>
+      </c>
+      <c r="D241">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>5</v>
+      </c>
+      <c r="B242" t="s">
+        <v>4</v>
+      </c>
+      <c r="C242">
+        <v>260</v>
+      </c>
+      <c r="D242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>5</v>
+      </c>
+      <c r="B243" t="s">
+        <v>5</v>
+      </c>
+      <c r="C243">
+        <v>260</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>6</v>
+      </c>
+      <c r="B244" t="s">
+        <v>4</v>
+      </c>
+      <c r="C244">
+        <v>260</v>
+      </c>
+      <c r="D244">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>6</v>
+      </c>
+      <c r="B245" t="s">
+        <v>5</v>
+      </c>
+      <c r="C245">
+        <v>260</v>
+      </c>
+      <c r="D245">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>7</v>
+      </c>
+      <c r="B246" t="s">
+        <v>4</v>
+      </c>
+      <c r="C246">
+        <v>260</v>
+      </c>
+      <c r="D246">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>7</v>
+      </c>
+      <c r="B247" t="s">
+        <v>5</v>
+      </c>
+      <c r="C247">
+        <v>260</v>
+      </c>
+      <c r="D247">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>8</v>
+      </c>
+      <c r="B248" t="s">
+        <v>4</v>
+      </c>
+      <c r="C248">
+        <v>260</v>
+      </c>
+      <c r="D248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>8</v>
+      </c>
+      <c r="B249" t="s">
+        <v>5</v>
+      </c>
+      <c r="C249">
+        <v>260</v>
+      </c>
+      <c r="D249">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>9</v>
+      </c>
+      <c r="B250" t="s">
+        <v>4</v>
+      </c>
+      <c r="C250">
+        <v>260</v>
+      </c>
+      <c r="D250">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>9</v>
+      </c>
+      <c r="B251" t="s">
+        <v>5</v>
+      </c>
+      <c r="C251">
+        <v>260</v>
+      </c>
+      <c r="D251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>10</v>
+      </c>
+      <c r="B252" t="s">
+        <v>4</v>
+      </c>
+      <c r="C252">
+        <v>260</v>
+      </c>
+      <c r="D252">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>10</v>
+      </c>
+      <c r="B253" t="s">
+        <v>5</v>
+      </c>
+      <c r="C253">
+        <v>260</v>
+      </c>
+      <c r="D253">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>11</v>
+      </c>
+      <c r="B254" t="s">
+        <v>4</v>
+      </c>
+      <c r="C254">
+        <v>260</v>
+      </c>
+      <c r="D254">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>11</v>
+      </c>
+      <c r="B255" t="s">
+        <v>5</v>
+      </c>
+      <c r="C255">
+        <v>260</v>
+      </c>
+      <c r="D255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>12</v>
+      </c>
+      <c r="B256" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256">
+        <v>260</v>
+      </c>
+      <c r="D256">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>12</v>
+      </c>
+      <c r="B257" t="s">
+        <v>5</v>
+      </c>
+      <c r="C257">
+        <v>260</v>
+      </c>
+      <c r="D257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>13</v>
+      </c>
+      <c r="B258" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258">
+        <v>260</v>
+      </c>
+      <c r="D258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>13</v>
+      </c>
+      <c r="B259" t="s">
+        <v>5</v>
+      </c>
+      <c r="C259">
+        <v>260</v>
+      </c>
+      <c r="D259">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>14</v>
+      </c>
+      <c r="B260" t="s">
+        <v>4</v>
+      </c>
+      <c r="C260">
+        <v>260</v>
+      </c>
+      <c r="D260">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>14</v>
+      </c>
+      <c r="B261" t="s">
+        <v>5</v>
+      </c>
+      <c r="C261">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>15</v>
+      </c>
+      <c r="B262" t="s">
+        <v>5</v>
+      </c>
+      <c r="C262">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>